<commit_message>
Added region_lang to Rmd and fixed bug where higher level category was not being filtered out
</commit_message>
<xml_diff>
--- a/inst/extdata/can_lang.xlsx
+++ b/inst/extdata/can_lang.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -435,9 +435,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nisga'a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-official languages</t>
   </si>
   <si>
     <t xml:space="preserve">North Slavey (Hare)</t>
@@ -3677,22 +3674,22 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B134" t="s">
         <v>141</v>
       </c>
       <c r="C134" t="n">
-        <v>7321060</v>
+        <v>765</v>
       </c>
       <c r="D134" t="n">
-        <v>3997195</v>
+        <v>340</v>
       </c>
       <c r="E134" t="n">
-        <v>275435</v>
+        <v>95</v>
       </c>
       <c r="F134" t="n">
-        <v>9369280</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="135">
@@ -3703,16 +3700,16 @@
         <v>142</v>
       </c>
       <c r="C135" t="n">
-        <v>765</v>
+        <v>315</v>
       </c>
       <c r="D135" t="n">
-        <v>340</v>
+        <v>110</v>
       </c>
       <c r="E135" t="n">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="F135" t="n">
-        <v>1005</v>
+        <v>550</v>
       </c>
     </row>
     <row r="136">
@@ -3723,56 +3720,56 @@
         <v>143</v>
       </c>
       <c r="C136" t="n">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="D136" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="E136" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>550</v>
+        <v>280</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B137" t="s">
         <v>144</v>
       </c>
       <c r="C137" t="n">
-        <v>220</v>
+        <v>4615</v>
       </c>
       <c r="D137" t="n">
-        <v>30</v>
+        <v>350</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F137" t="n">
-        <v>280</v>
+        <v>8120</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B138" t="s">
         <v>145</v>
       </c>
       <c r="C138" t="n">
-        <v>4615</v>
+        <v>280</v>
       </c>
       <c r="D138" t="n">
-        <v>350</v>
+        <v>30</v>
       </c>
       <c r="E138" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F138" t="n">
-        <v>8120</v>
+        <v>560</v>
       </c>
     </row>
     <row r="139">
@@ -3783,16 +3780,16 @@
         <v>146</v>
       </c>
       <c r="C139" t="n">
-        <v>280</v>
+        <v>12855</v>
       </c>
       <c r="D139" t="n">
-        <v>30</v>
+        <v>7905</v>
       </c>
       <c r="E139" t="n">
-        <v>10</v>
+        <v>1080</v>
       </c>
       <c r="F139" t="n">
-        <v>560</v>
+        <v>15605</v>
       </c>
     </row>
     <row r="140">
@@ -3803,16 +3800,16 @@
         <v>147</v>
       </c>
       <c r="C140" t="n">
-        <v>12855</v>
+        <v>17885</v>
       </c>
       <c r="D140" t="n">
-        <v>7905</v>
+        <v>6175</v>
       </c>
       <c r="E140" t="n">
-        <v>1080</v>
+        <v>765</v>
       </c>
       <c r="F140" t="n">
-        <v>15605</v>
+        <v>28580</v>
       </c>
     </row>
     <row r="141">
@@ -3823,16 +3820,16 @@
         <v>148</v>
       </c>
       <c r="C141" t="n">
-        <v>17885</v>
+        <v>275</v>
       </c>
       <c r="D141" t="n">
-        <v>6175</v>
+        <v>80</v>
       </c>
       <c r="E141" t="n">
-        <v>765</v>
+        <v>20</v>
       </c>
       <c r="F141" t="n">
-        <v>28580</v>
+        <v>820</v>
       </c>
     </row>
     <row r="142">
@@ -3843,36 +3840,36 @@
         <v>149</v>
       </c>
       <c r="C142" t="n">
-        <v>275</v>
+        <v>60</v>
       </c>
       <c r="D142" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E142" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>820</v>
+        <v>185</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B143" t="s">
         <v>150</v>
       </c>
       <c r="C143" t="n">
-        <v>60</v>
+        <v>1055</v>
       </c>
       <c r="D143" t="n">
-        <v>15</v>
+        <v>475</v>
       </c>
       <c r="E143" t="n">
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>185</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="144">
@@ -3883,16 +3880,16 @@
         <v>151</v>
       </c>
       <c r="C144" t="n">
-        <v>1055</v>
+        <v>4960</v>
       </c>
       <c r="D144" t="n">
-        <v>475</v>
+        <v>3410</v>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F144" t="n">
-        <v>1530</v>
+        <v>6245</v>
       </c>
     </row>
     <row r="145">
@@ -3903,56 +3900,56 @@
         <v>152</v>
       </c>
       <c r="C145" t="n">
-        <v>4960</v>
+        <v>3685</v>
       </c>
       <c r="D145" t="n">
-        <v>3410</v>
+        <v>1110</v>
       </c>
       <c r="E145" t="n">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="F145" t="n">
-        <v>6245</v>
+        <v>9730</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B146" t="s">
         <v>153</v>
       </c>
       <c r="C146" t="n">
-        <v>3685</v>
+        <v>150</v>
       </c>
       <c r="D146" t="n">
-        <v>1110</v>
+        <v>75</v>
       </c>
       <c r="E146" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>9730</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B147" t="s">
         <v>154</v>
       </c>
       <c r="C147" t="n">
-        <v>150</v>
+        <v>4045</v>
       </c>
       <c r="D147" t="n">
-        <v>75</v>
+        <v>1200</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F147" t="n">
-        <v>205</v>
+        <v>5425</v>
       </c>
     </row>
     <row r="148">
@@ -3963,16 +3960,16 @@
         <v>155</v>
       </c>
       <c r="C148" t="n">
-        <v>4045</v>
+        <v>1390</v>
       </c>
       <c r="D148" t="n">
-        <v>1200</v>
+        <v>240</v>
       </c>
       <c r="E148" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>5425</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="149">
@@ -3983,16 +3980,16 @@
         <v>156</v>
       </c>
       <c r="C149" t="n">
-        <v>1390</v>
+        <v>16905</v>
       </c>
       <c r="D149" t="n">
-        <v>240</v>
+        <v>10590</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F149" t="n">
-        <v>1800</v>
+        <v>23180</v>
       </c>
     </row>
     <row r="150">
@@ -4003,56 +4000,56 @@
         <v>157</v>
       </c>
       <c r="C150" t="n">
-        <v>16905</v>
+        <v>214200</v>
       </c>
       <c r="D150" t="n">
-        <v>10590</v>
+        <v>143025</v>
       </c>
       <c r="E150" t="n">
-        <v>50</v>
+        <v>4580</v>
       </c>
       <c r="F150" t="n">
-        <v>23180</v>
+        <v>252325</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B151" t="s">
         <v>158</v>
       </c>
       <c r="C151" t="n">
-        <v>214200</v>
+        <v>3065</v>
       </c>
       <c r="D151" t="n">
-        <v>143025</v>
+        <v>1345</v>
       </c>
       <c r="E151" t="n">
-        <v>4580</v>
+        <v>95</v>
       </c>
       <c r="F151" t="n">
-        <v>252325</v>
+        <v>5905</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B152" t="s">
         <v>159</v>
       </c>
       <c r="C152" t="n">
-        <v>3065</v>
+        <v>181710</v>
       </c>
       <c r="D152" t="n">
-        <v>1345</v>
+        <v>74780</v>
       </c>
       <c r="E152" t="n">
-        <v>95</v>
+        <v>2495</v>
       </c>
       <c r="F152" t="n">
-        <v>5905</v>
+        <v>214965</v>
       </c>
     </row>
     <row r="153">
@@ -4063,16 +4060,16 @@
         <v>160</v>
       </c>
       <c r="C153" t="n">
-        <v>181710</v>
+        <v>221535</v>
       </c>
       <c r="D153" t="n">
-        <v>74780</v>
+        <v>98710</v>
       </c>
       <c r="E153" t="n">
-        <v>2495</v>
+        <v>7485</v>
       </c>
       <c r="F153" t="n">
-        <v>214965</v>
+        <v>295955</v>
       </c>
     </row>
     <row r="154">
@@ -4083,16 +4080,16 @@
         <v>161</v>
       </c>
       <c r="C154" t="n">
-        <v>221535</v>
+        <v>501680</v>
       </c>
       <c r="D154" t="n">
-        <v>98710</v>
+        <v>349140</v>
       </c>
       <c r="E154" t="n">
-        <v>7485</v>
+        <v>27865</v>
       </c>
       <c r="F154" t="n">
-        <v>295955</v>
+        <v>668240</v>
       </c>
     </row>
     <row r="155">
@@ -4103,16 +4100,16 @@
         <v>162</v>
       </c>
       <c r="C155" t="n">
-        <v>501680</v>
+        <v>695</v>
       </c>
       <c r="D155" t="n">
-        <v>349140</v>
+        <v>730</v>
       </c>
       <c r="E155" t="n">
-        <v>27865</v>
+        <v>130</v>
       </c>
       <c r="F155" t="n">
-        <v>668240</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="156">
@@ -4123,16 +4120,16 @@
         <v>163</v>
       </c>
       <c r="C156" t="n">
-        <v>695</v>
+        <v>96660</v>
       </c>
       <c r="D156" t="n">
-        <v>730</v>
+        <v>53325</v>
       </c>
       <c r="E156" t="n">
-        <v>130</v>
+        <v>745</v>
       </c>
       <c r="F156" t="n">
-        <v>4665</v>
+        <v>115050</v>
       </c>
     </row>
     <row r="157">
@@ -4143,16 +4140,16 @@
         <v>164</v>
       </c>
       <c r="C157" t="n">
-        <v>96660</v>
+        <v>5850</v>
       </c>
       <c r="D157" t="n">
-        <v>53325</v>
+        <v>2110</v>
       </c>
       <c r="E157" t="n">
-        <v>745</v>
+        <v>0</v>
       </c>
       <c r="F157" t="n">
-        <v>115050</v>
+        <v>8590</v>
       </c>
     </row>
     <row r="158">
@@ -4163,36 +4160,36 @@
         <v>165</v>
       </c>
       <c r="C158" t="n">
-        <v>5850</v>
+        <v>188255</v>
       </c>
       <c r="D158" t="n">
-        <v>2110</v>
+        <v>116595</v>
       </c>
       <c r="E158" t="n">
-        <v>0</v>
+        <v>4855</v>
       </c>
       <c r="F158" t="n">
-        <v>8590</v>
+        <v>269645</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B159" t="s">
         <v>166</v>
       </c>
       <c r="C159" t="n">
-        <v>188255</v>
+        <v>260</v>
       </c>
       <c r="D159" t="n">
-        <v>116595</v>
+        <v>25</v>
       </c>
       <c r="E159" t="n">
-        <v>4855</v>
+        <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>269645</v>
+        <v>560</v>
       </c>
     </row>
     <row r="160">
@@ -4203,76 +4200,76 @@
         <v>167</v>
       </c>
       <c r="C160" t="n">
-        <v>260</v>
+        <v>80</v>
       </c>
       <c r="D160" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
       </c>
       <c r="F160" t="n">
-        <v>560</v>
+        <v>145</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B161" t="s">
         <v>168</v>
       </c>
       <c r="C161" t="n">
-        <v>80</v>
+        <v>1090</v>
       </c>
       <c r="D161" t="n">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F161" t="n">
-        <v>145</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B162" t="s">
         <v>169</v>
       </c>
       <c r="C162" t="n">
-        <v>1090</v>
+        <v>85</v>
       </c>
       <c r="D162" t="n">
-        <v>190</v>
+        <v>15</v>
       </c>
       <c r="E162" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>3980</v>
+        <v>185</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B163" t="s">
         <v>170</v>
       </c>
       <c r="C163" t="n">
-        <v>85</v>
+        <v>2150</v>
       </c>
       <c r="D163" t="n">
-        <v>15</v>
+        <v>1205</v>
       </c>
       <c r="E163" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F163" t="n">
-        <v>185</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="164">
@@ -4283,16 +4280,16 @@
         <v>171</v>
       </c>
       <c r="C164" t="n">
-        <v>2150</v>
+        <v>57350</v>
       </c>
       <c r="D164" t="n">
-        <v>1205</v>
+        <v>31750</v>
       </c>
       <c r="E164" t="n">
-        <v>65</v>
+        <v>530</v>
       </c>
       <c r="F164" t="n">
-        <v>3220</v>
+        <v>73780</v>
       </c>
     </row>
     <row r="165">
@@ -4303,16 +4300,16 @@
         <v>172</v>
       </c>
       <c r="C165" t="n">
-        <v>57350</v>
+        <v>9550</v>
       </c>
       <c r="D165" t="n">
-        <v>31750</v>
+        <v>3890</v>
       </c>
       <c r="E165" t="n">
-        <v>530</v>
+        <v>30</v>
       </c>
       <c r="F165" t="n">
-        <v>73780</v>
+        <v>11275</v>
       </c>
     </row>
     <row r="166">
@@ -4323,56 +4320,56 @@
         <v>173</v>
       </c>
       <c r="C166" t="n">
-        <v>9550</v>
+        <v>3185</v>
       </c>
       <c r="D166" t="n">
-        <v>3890</v>
+        <v>1035</v>
       </c>
       <c r="E166" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>11275</v>
+        <v>5430</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B167" t="s">
         <v>174</v>
       </c>
       <c r="C167" t="n">
-        <v>3185</v>
+        <v>445</v>
       </c>
       <c r="D167" t="n">
-        <v>1035</v>
+        <v>50</v>
       </c>
       <c r="E167" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F167" t="n">
-        <v>5430</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B168" t="s">
         <v>175</v>
       </c>
       <c r="C168" t="n">
-        <v>445</v>
+        <v>4125</v>
       </c>
       <c r="D168" t="n">
-        <v>50</v>
+        <v>6690</v>
       </c>
       <c r="E168" t="n">
-        <v>35</v>
+        <v>645</v>
       </c>
       <c r="F168" t="n">
-        <v>1305</v>
+        <v>22280</v>
       </c>
     </row>
     <row r="169">
@@ -4383,16 +4380,16 @@
         <v>176</v>
       </c>
       <c r="C169" t="n">
-        <v>4125</v>
+        <v>11860</v>
       </c>
       <c r="D169" t="n">
-        <v>6690</v>
+        <v>4975</v>
       </c>
       <c r="E169" t="n">
-        <v>645</v>
+        <v>35</v>
       </c>
       <c r="F169" t="n">
-        <v>22280</v>
+        <v>20260</v>
       </c>
     </row>
     <row r="170">
@@ -4403,36 +4400,36 @@
         <v>177</v>
       </c>
       <c r="C170" t="n">
-        <v>11860</v>
+        <v>16335</v>
       </c>
       <c r="D170" t="n">
-        <v>4975</v>
+        <v>7790</v>
       </c>
       <c r="E170" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F170" t="n">
-        <v>20260</v>
+        <v>27825</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B171" t="s">
         <v>178</v>
       </c>
       <c r="C171" t="n">
-        <v>16335</v>
+        <v>55</v>
       </c>
       <c r="D171" t="n">
-        <v>7790</v>
+        <v>20</v>
       </c>
       <c r="E171" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>27825</v>
+        <v>140</v>
       </c>
     </row>
     <row r="172">
@@ -4443,36 +4440,36 @@
         <v>179</v>
       </c>
       <c r="C172" t="n">
-        <v>55</v>
+        <v>280</v>
       </c>
       <c r="D172" t="n">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="E172" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F172" t="n">
-        <v>140</v>
+        <v>675</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B173" t="s">
         <v>180</v>
       </c>
       <c r="C173" t="n">
-        <v>280</v>
+        <v>2420</v>
       </c>
       <c r="D173" t="n">
-        <v>105</v>
+        <v>670</v>
       </c>
       <c r="E173" t="n">
         <v>10</v>
       </c>
       <c r="F173" t="n">
-        <v>675</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="174">
@@ -4483,16 +4480,16 @@
         <v>181</v>
       </c>
       <c r="C174" t="n">
-        <v>2420</v>
+        <v>17580</v>
       </c>
       <c r="D174" t="n">
-        <v>670</v>
+        <v>5610</v>
       </c>
       <c r="E174" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F174" t="n">
-        <v>2995</v>
+        <v>21470</v>
       </c>
     </row>
     <row r="175">
@@ -4503,16 +4500,16 @@
         <v>182</v>
       </c>
       <c r="C175" t="n">
-        <v>17580</v>
+        <v>9785</v>
       </c>
       <c r="D175" t="n">
-        <v>5610</v>
+        <v>2055</v>
       </c>
       <c r="E175" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="F175" t="n">
-        <v>21470</v>
+        <v>11490</v>
       </c>
     </row>
     <row r="176">
@@ -4523,36 +4520,36 @@
         <v>183</v>
       </c>
       <c r="C176" t="n">
-        <v>9785</v>
+        <v>36755</v>
       </c>
       <c r="D176" t="n">
-        <v>2055</v>
+        <v>22895</v>
       </c>
       <c r="E176" t="n">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="F176" t="n">
-        <v>11490</v>
+        <v>49660</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B177" t="s">
         <v>184</v>
       </c>
       <c r="C177" t="n">
-        <v>36755</v>
+        <v>945</v>
       </c>
       <c r="D177" t="n">
-        <v>22895</v>
+        <v>370</v>
       </c>
       <c r="E177" t="n">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="F177" t="n">
-        <v>49660</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="178">
@@ -4563,16 +4560,16 @@
         <v>185</v>
       </c>
       <c r="C178" t="n">
-        <v>945</v>
+        <v>45</v>
       </c>
       <c r="D178" t="n">
-        <v>370</v>
+        <v>15</v>
       </c>
       <c r="E178" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>1365</v>
+        <v>40</v>
       </c>
     </row>
     <row r="179">
@@ -4583,56 +4580,56 @@
         <v>186</v>
       </c>
       <c r="C179" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="D179" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E179" t="n">
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>40</v>
+        <v>145</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B180" t="s">
         <v>187</v>
       </c>
       <c r="C180" t="n">
-        <v>70</v>
+        <v>458850</v>
       </c>
       <c r="D180" t="n">
-        <v>5</v>
+        <v>263505</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>13030</v>
       </c>
       <c r="F180" t="n">
-        <v>145</v>
+        <v>995260</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B181" t="s">
         <v>188</v>
       </c>
       <c r="C181" t="n">
-        <v>458850</v>
+        <v>40</v>
       </c>
       <c r="D181" t="n">
-        <v>263505</v>
+        <v>5</v>
       </c>
       <c r="E181" t="n">
-        <v>13030</v>
+        <v>10</v>
       </c>
       <c r="F181" t="n">
-        <v>995260</v>
+        <v>285</v>
       </c>
     </row>
     <row r="182">
@@ -4643,16 +4640,16 @@
         <v>189</v>
       </c>
       <c r="C182" t="n">
-        <v>40</v>
+        <v>3025</v>
       </c>
       <c r="D182" t="n">
-        <v>5</v>
+        <v>1950</v>
       </c>
       <c r="E182" t="n">
-        <v>10</v>
+        <v>240</v>
       </c>
       <c r="F182" t="n">
-        <v>285</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="183">
@@ -4663,76 +4660,76 @@
         <v>190</v>
       </c>
       <c r="C183" t="n">
-        <v>3025</v>
+        <v>80</v>
       </c>
       <c r="D183" t="n">
-        <v>1950</v>
+        <v>25</v>
       </c>
       <c r="E183" t="n">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="F183" t="n">
-        <v>3675</v>
+        <v>365</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B184" t="s">
         <v>191</v>
       </c>
       <c r="C184" t="n">
+        <v>13370</v>
+      </c>
+      <c r="D184" t="n">
+        <v>5370</v>
+      </c>
+      <c r="E184" t="n">
         <v>80</v>
       </c>
-      <c r="D184" t="n">
-        <v>25</v>
-      </c>
-      <c r="E184" t="n">
-        <v>15</v>
-      </c>
       <c r="F184" t="n">
-        <v>365</v>
+        <v>38685</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B185" t="s">
         <v>192</v>
       </c>
       <c r="C185" t="n">
-        <v>13370</v>
+        <v>1440</v>
       </c>
       <c r="D185" t="n">
-        <v>5370</v>
+        <v>330</v>
       </c>
       <c r="E185" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F185" t="n">
-        <v>38685</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B186" t="s">
         <v>193</v>
       </c>
       <c r="C186" t="n">
-        <v>1440</v>
+        <v>6840</v>
       </c>
       <c r="D186" t="n">
-        <v>330</v>
+        <v>1050</v>
       </c>
       <c r="E186" t="n">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="F186" t="n">
-        <v>2350</v>
+        <v>14140</v>
       </c>
     </row>
     <row r="187">
@@ -4743,56 +4740,56 @@
         <v>194</v>
       </c>
       <c r="C187" t="n">
-        <v>6840</v>
+        <v>431385</v>
       </c>
       <c r="D187" t="n">
-        <v>1050</v>
+        <v>213790</v>
       </c>
       <c r="E187" t="n">
-        <v>125</v>
+        <v>3450</v>
       </c>
       <c r="F187" t="n">
-        <v>14140</v>
+        <v>612735</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B188" t="s">
         <v>195</v>
       </c>
       <c r="C188" t="n">
-        <v>431385</v>
+        <v>95</v>
       </c>
       <c r="D188" t="n">
-        <v>213790</v>
+        <v>5</v>
       </c>
       <c r="E188" t="n">
-        <v>3450</v>
+        <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>612735</v>
+        <v>265</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B189" t="s">
         <v>196</v>
       </c>
       <c r="C189" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D189" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E189" t="n">
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>265</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190">
@@ -4803,16 +4800,16 @@
         <v>197</v>
       </c>
       <c r="C190" t="n">
-        <v>85</v>
+        <v>140720</v>
       </c>
       <c r="D190" t="n">
-        <v>30</v>
+        <v>96955</v>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>2085</v>
       </c>
       <c r="F190" t="n">
-        <v>115</v>
+        <v>189860</v>
       </c>
     </row>
     <row r="191">
@@ -4823,16 +4820,16 @@
         <v>198</v>
       </c>
       <c r="C191" t="n">
-        <v>140720</v>
+        <v>15660</v>
       </c>
       <c r="D191" t="n">
-        <v>96955</v>
+        <v>8280</v>
       </c>
       <c r="E191" t="n">
-        <v>2085</v>
+        <v>40</v>
       </c>
       <c r="F191" t="n">
-        <v>189860</v>
+        <v>23165</v>
       </c>
     </row>
     <row r="192">
@@ -4843,56 +4840,56 @@
         <v>199</v>
       </c>
       <c r="C192" t="n">
-        <v>15660</v>
+        <v>9255</v>
       </c>
       <c r="D192" t="n">
-        <v>8280</v>
+        <v>3365</v>
       </c>
       <c r="E192" t="n">
-        <v>40</v>
+        <v>525</v>
       </c>
       <c r="F192" t="n">
-        <v>23165</v>
+        <v>15395</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B193" t="s">
         <v>200</v>
       </c>
       <c r="C193" t="n">
-        <v>9255</v>
+        <v>335</v>
       </c>
       <c r="D193" t="n">
-        <v>3365</v>
+        <v>20</v>
       </c>
       <c r="E193" t="n">
-        <v>525</v>
+        <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>15395</v>
+        <v>450</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B194" t="s">
         <v>201</v>
       </c>
       <c r="C194" t="n">
-        <v>335</v>
+        <v>6160</v>
       </c>
       <c r="D194" t="n">
-        <v>20</v>
+        <v>4590</v>
       </c>
       <c r="E194" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F194" t="n">
-        <v>450</v>
+        <v>7050</v>
       </c>
     </row>
     <row r="195">
@@ -4903,16 +4900,16 @@
         <v>202</v>
       </c>
       <c r="C195" t="n">
-        <v>6160</v>
+        <v>1405</v>
       </c>
       <c r="D195" t="n">
-        <v>4590</v>
+        <v>655</v>
       </c>
       <c r="E195" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F195" t="n">
-        <v>7050</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="196">
@@ -4923,36 +4920,36 @@
         <v>203</v>
       </c>
       <c r="C196" t="n">
-        <v>1405</v>
+        <v>16645</v>
       </c>
       <c r="D196" t="n">
-        <v>655</v>
+        <v>10205</v>
       </c>
       <c r="E196" t="n">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="F196" t="n">
-        <v>2380</v>
+        <v>21340</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B197" t="s">
         <v>204</v>
       </c>
       <c r="C197" t="n">
-        <v>16645</v>
+        <v>95</v>
       </c>
       <c r="D197" t="n">
-        <v>10205</v>
+        <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="F197" t="n">
-        <v>21340</v>
+        <v>260</v>
       </c>
     </row>
     <row r="198">
@@ -4963,36 +4960,36 @@
         <v>205</v>
       </c>
       <c r="C198" t="n">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="D198" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E198" t="n">
         <v>10</v>
       </c>
       <c r="F198" t="n">
-        <v>260</v>
+        <v>410</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B199" t="s">
         <v>206</v>
       </c>
       <c r="C199" t="n">
-        <v>200</v>
+        <v>1315</v>
       </c>
       <c r="D199" t="n">
-        <v>30</v>
+        <v>455</v>
       </c>
       <c r="E199" t="n">
         <v>10</v>
       </c>
       <c r="F199" t="n">
-        <v>410</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="200">
@@ -5003,16 +5000,16 @@
         <v>207</v>
       </c>
       <c r="C200" t="n">
-        <v>1315</v>
+        <v>32815</v>
       </c>
       <c r="D200" t="n">
-        <v>455</v>
+        <v>18955</v>
       </c>
       <c r="E200" t="n">
-        <v>10</v>
+        <v>690</v>
       </c>
       <c r="F200" t="n">
-        <v>1875</v>
+        <v>50770</v>
       </c>
     </row>
     <row r="201">
@@ -5023,16 +5020,16 @@
         <v>208</v>
       </c>
       <c r="C201" t="n">
-        <v>32815</v>
+        <v>102485</v>
       </c>
       <c r="D201" t="n">
-        <v>18955</v>
+        <v>28250</v>
       </c>
       <c r="E201" t="n">
-        <v>690</v>
+        <v>1210</v>
       </c>
       <c r="F201" t="n">
-        <v>50770</v>
+        <v>132115</v>
       </c>
     </row>
     <row r="202">
@@ -5043,16 +5040,16 @@
         <v>209</v>
       </c>
       <c r="C202" t="n">
-        <v>102485</v>
+        <v>10</v>
       </c>
       <c r="D202" t="n">
-        <v>28250</v>
+        <v>5</v>
       </c>
       <c r="E202" t="n">
-        <v>1210</v>
+        <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>132115</v>
+        <v>25</v>
       </c>
     </row>
     <row r="203">
@@ -5063,16 +5060,16 @@
         <v>210</v>
       </c>
       <c r="C203" t="n">
-        <v>10</v>
+        <v>210815</v>
       </c>
       <c r="D203" t="n">
-        <v>5</v>
+        <v>128785</v>
       </c>
       <c r="E203" t="n">
-        <v>0</v>
+        <v>1495</v>
       </c>
       <c r="F203" t="n">
-        <v>25</v>
+        <v>322220</v>
       </c>
     </row>
     <row r="204">
@@ -5083,16 +5080,16 @@
         <v>211</v>
       </c>
       <c r="C204" t="n">
-        <v>210815</v>
+        <v>1035</v>
       </c>
       <c r="D204" t="n">
-        <v>128785</v>
+        <v>610</v>
       </c>
       <c r="E204" t="n">
-        <v>1495</v>
+        <v>20</v>
       </c>
       <c r="F204" t="n">
-        <v>322220</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="205">
@@ -5103,16 +5100,16 @@
         <v>212</v>
       </c>
       <c r="C205" t="n">
-        <v>1035</v>
+        <v>1720</v>
       </c>
       <c r="D205" t="n">
-        <v>610</v>
+        <v>995</v>
       </c>
       <c r="E205" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F205" t="n">
-        <v>1390</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="206">
@@ -5123,16 +5120,16 @@
         <v>213</v>
       </c>
       <c r="C206" t="n">
-        <v>1720</v>
+        <v>156430</v>
       </c>
       <c r="D206" t="n">
-        <v>995</v>
+        <v>104245</v>
       </c>
       <c r="E206" t="n">
-        <v>15</v>
+        <v>8075</v>
       </c>
       <c r="F206" t="n">
-        <v>2465</v>
+        <v>198895</v>
       </c>
     </row>
     <row r="207">
@@ -5143,56 +5140,56 @@
         <v>214</v>
       </c>
       <c r="C207" t="n">
-        <v>156430</v>
+        <v>3895</v>
       </c>
       <c r="D207" t="n">
-        <v>104245</v>
+        <v>355</v>
       </c>
       <c r="E207" t="n">
-        <v>8075</v>
+        <v>35</v>
       </c>
       <c r="F207" t="n">
-        <v>198895</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B208" t="s">
         <v>215</v>
       </c>
       <c r="C208" t="n">
-        <v>3895</v>
+        <v>10</v>
       </c>
       <c r="D208" t="n">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E208" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F208" t="n">
-        <v>4400</v>
+        <v>25</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B209" t="s">
         <v>216</v>
       </c>
       <c r="C209" t="n">
-        <v>10</v>
+        <v>1110</v>
       </c>
       <c r="D209" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="E209" t="n">
         <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>25</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="210">
@@ -5203,16 +5200,16 @@
         <v>217</v>
       </c>
       <c r="C210" t="n">
-        <v>1110</v>
+        <v>1075</v>
       </c>
       <c r="D210" t="n">
-        <v>310</v>
+        <v>95</v>
       </c>
       <c r="E210" t="n">
         <v>0</v>
       </c>
       <c r="F210" t="n">
-        <v>1395</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="211">
@@ -5223,56 +5220,56 @@
         <v>218</v>
       </c>
       <c r="C211" t="n">
-        <v>1075</v>
+        <v>3990</v>
       </c>
       <c r="D211" t="n">
-        <v>95</v>
+        <v>1385</v>
       </c>
       <c r="E211" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F211" t="n">
-        <v>1695</v>
+        <v>8240</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B212" t="s">
         <v>219</v>
       </c>
       <c r="C212" t="n">
-        <v>3990</v>
+        <v>1840</v>
       </c>
       <c r="D212" t="n">
-        <v>1385</v>
+        <v>800</v>
       </c>
       <c r="E212" t="n">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F212" t="n">
-        <v>8240</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B213" t="s">
         <v>220</v>
       </c>
       <c r="C213" t="n">
-        <v>1840</v>
+        <v>12915</v>
       </c>
       <c r="D213" t="n">
-        <v>800</v>
+        <v>7650</v>
       </c>
       <c r="E213" t="n">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="F213" t="n">
-        <v>2665</v>
+        <v>16530</v>
       </c>
     </row>
     <row r="214">
@@ -5283,16 +5280,16 @@
         <v>221</v>
       </c>
       <c r="C214" t="n">
-        <v>12915</v>
+        <v>13555</v>
       </c>
       <c r="D214" t="n">
-        <v>7650</v>
+        <v>7085</v>
       </c>
       <c r="E214" t="n">
-        <v>105</v>
+        <v>895</v>
       </c>
       <c r="F214" t="n">
-        <v>16530</v>
+        <v>20985</v>
       </c>
     </row>
     <row r="215">
@@ -5303,35 +5300,15 @@
         <v>222</v>
       </c>
       <c r="C215" t="n">
-        <v>13555</v>
+        <v>9080</v>
       </c>
       <c r="D215" t="n">
-        <v>7085</v>
+        <v>2615</v>
       </c>
       <c r="E215" t="n">
-        <v>895</v>
+        <v>15</v>
       </c>
       <c r="F215" t="n">
-        <v>20985</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="s">
-        <v>8</v>
-      </c>
-      <c r="B216" t="s">
-        <v>223</v>
-      </c>
-      <c r="C216" t="n">
-        <v>9080</v>
-      </c>
-      <c r="D216" t="n">
-        <v>2615</v>
-      </c>
-      <c r="E216" t="n">
-        <v>15</v>
-      </c>
-      <c r="F216" t="n">
         <v>22415</v>
       </c>
     </row>

</xml_diff>